<commit_message>
düzenlemeler yapıldı, rapor eklendi
</commit_message>
<xml_diff>
--- a/data/lessons/YZM002/table1.xlsx
+++ b/data/lessons/YZM002/table1.xlsx
@@ -731,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5999999404625819</v>
+        <v>0.5999999999923434</v>
       </c>
     </row>
     <row r="14">
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.399999960308388</v>
+        <v>0.3999999999948956</v>
       </c>
     </row>
     <row r="15">
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.399999960308388</v>
+        <v>0.3999999999948956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>